<commit_message>
Add DCF valuation, market data, proofreading section, and model modification guide
- Added DCF Valuation section with discount rate and terminal growth inputs
- Added Market Data & Comparison section with upside/downside calculation
- Added Data Sources & SEC Filing reference section in model
- Added Proofreading & Verification protocol to CLAUDE_MODELING_GUIDE.md
- Added Instructions for Efficient Model Modifications section for Claude
- Added gray shading to CapEx % and D&A % driver rows
- Verified Q3 2024 data against SEC filings (revenue, segments match)
- Updated checklist with DCF and market data items

https://claude.ai/code/session_017T6i5yR8r72YUrVTHRiVvx
</commit_message>
<xml_diff>
--- a/AMN_Healthcare_Model_v4.xlsx
+++ b/AMN_Healthcare_Model_v4.xlsx
@@ -16,9 +16,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0x"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="$#,##0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -40,7 +43,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -51,6 +54,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00F0F0F0"/>
         <bgColor rgb="00F0F0F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E6F3FF"/>
+        <bgColor rgb="00E6F3FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -66,7 +75,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -76,6 +85,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -441,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC157"/>
+  <dimension ref="A1:AC207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4206,20 +4222,20 @@
       </c>
     </row>
     <row r="85">
-      <c r="B85" t="inlineStr">
+      <c r="B85" s="6" t="inlineStr">
         <is>
           <t>CapEx as % of Revenue</t>
         </is>
       </c>
-      <c r="D85" s="4">
+      <c r="D85" s="7">
         <f>D83/D84</f>
         <v/>
       </c>
-      <c r="E85" s="4">
+      <c r="E85" s="7">
         <f>E83/E84</f>
         <v/>
       </c>
-      <c r="F85" s="4">
+      <c r="F85" s="7">
         <f>F83/F84</f>
         <v/>
       </c>
@@ -4244,20 +4260,20 @@
       </c>
     </row>
     <row r="88">
-      <c r="B88" t="inlineStr">
+      <c r="B88" s="6" t="inlineStr">
         <is>
           <t>D&amp;A as % of Revenue</t>
         </is>
       </c>
-      <c r="D88" s="4">
+      <c r="D88" s="7">
         <f>D87/D84</f>
         <v/>
       </c>
-      <c r="E88" s="4">
+      <c r="E88" s="7">
         <f>E87/E84</f>
         <v/>
       </c>
-      <c r="F88" s="4">
+      <c r="F88" s="7">
         <f>F87/F84</f>
         <v/>
       </c>
@@ -5993,6 +6009,579 @@
       <c r="F157" s="3">
         <f>F154-F156</f>
         <v/>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B160" s="2" t="inlineStr">
+        <is>
+          <t>DCF VALUATION - Annual (in Thousands USD)</t>
+        </is>
+      </c>
+      <c r="G160" s="2" t="inlineStr">
+        <is>
+          <t>FY 2025</t>
+        </is>
+      </c>
+      <c r="H160" s="2" t="inlineStr">
+        <is>
+          <t>FY 2026</t>
+        </is>
+      </c>
+      <c r="I160" s="2" t="inlineStr">
+        <is>
+          <t>FY 2027</t>
+        </is>
+      </c>
+      <c r="J160" s="2" t="inlineStr">
+        <is>
+          <t>FY 2028</t>
+        </is>
+      </c>
+      <c r="K160" s="2" t="inlineStr">
+        <is>
+          <t>FY 2029</t>
+        </is>
+      </c>
+      <c r="L160" s="2" t="inlineStr">
+        <is>
+          <t>FY 2030</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="B161" s="2" t="inlineStr">
+        <is>
+          <t>INPUTS</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="B162" s="9" t="inlineStr">
+        <is>
+          <t>Discount Rate (WACC)</t>
+        </is>
+      </c>
+      <c r="G162" s="10" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="B163" s="9" t="inlineStr">
+        <is>
+          <t>Terminal Growth Rate</t>
+        </is>
+      </c>
+      <c r="G163" s="10" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="B165" s="2" t="inlineStr">
+        <is>
+          <t>FREE CASH FLOW</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>EBITDA</t>
+        </is>
+      </c>
+      <c r="G166" s="3">
+        <f>G31</f>
+        <v/>
+      </c>
+      <c r="H166" s="3">
+        <f>H31</f>
+        <v/>
+      </c>
+      <c r="I166" s="3">
+        <f>I31</f>
+        <v/>
+      </c>
+      <c r="J166" s="3">
+        <f>J31</f>
+        <v/>
+      </c>
+      <c r="K166" s="3">
+        <f>K31</f>
+        <v/>
+      </c>
+      <c r="L166" s="3">
+        <f>L31</f>
+        <v/>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>- D&amp;A (add back already in EBITDA)</t>
+        </is>
+      </c>
+      <c r="G167" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H167" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I167" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J167" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K167" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L167" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>- CapEx (as % of Revenue)</t>
+        </is>
+      </c>
+      <c r="G168" s="3">
+        <f>-G16*F85</f>
+        <v/>
+      </c>
+      <c r="H168" s="3">
+        <f>-H16*F85</f>
+        <v/>
+      </c>
+      <c r="I168" s="3">
+        <f>-I16*F85</f>
+        <v/>
+      </c>
+      <c r="J168" s="3">
+        <f>-J16*F85</f>
+        <v/>
+      </c>
+      <c r="K168" s="3">
+        <f>-K16*F85</f>
+        <v/>
+      </c>
+      <c r="L168" s="3">
+        <f>-L16*F85</f>
+        <v/>
+      </c>
+    </row>
+    <row r="169">
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>- Change in NWC (assumed 0)</t>
+        </is>
+      </c>
+      <c r="G169" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H169" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I169" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J169" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K169" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L169" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>- Cash Taxes</t>
+        </is>
+      </c>
+      <c r="G170" s="3">
+        <f>-G27</f>
+        <v/>
+      </c>
+      <c r="H170" s="3">
+        <f>-H27</f>
+        <v/>
+      </c>
+      <c r="I170" s="3">
+        <f>-I27</f>
+        <v/>
+      </c>
+      <c r="J170" s="3">
+        <f>-J27</f>
+        <v/>
+      </c>
+      <c r="K170" s="3">
+        <f>-K27</f>
+        <v/>
+      </c>
+      <c r="L170" s="3">
+        <f>-L27</f>
+        <v/>
+      </c>
+    </row>
+    <row r="171">
+      <c r="B171" s="5" t="inlineStr">
+        <is>
+          <t>Free Cash Flow</t>
+        </is>
+      </c>
+      <c r="G171" s="3">
+        <f>G166+G168+G169+G170</f>
+        <v/>
+      </c>
+      <c r="H171" s="3">
+        <f>H166+H168+H169+H170</f>
+        <v/>
+      </c>
+      <c r="I171" s="3">
+        <f>I166+I168+I169+I170</f>
+        <v/>
+      </c>
+      <c r="J171" s="3">
+        <f>J166+J168+J169+J170</f>
+        <v/>
+      </c>
+      <c r="K171" s="3">
+        <f>K166+K168+K169+K170</f>
+        <v/>
+      </c>
+      <c r="L171" s="3">
+        <f>L166+L168+L169+L170</f>
+        <v/>
+      </c>
+    </row>
+    <row r="173">
+      <c r="B173" s="2" t="inlineStr">
+        <is>
+          <t>PRESENT VALUE</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Discount Factor</t>
+        </is>
+      </c>
+      <c r="G174" s="11">
+        <f>1/(1+$G$162)^1</f>
+        <v/>
+      </c>
+      <c r="H174" s="11">
+        <f>1/(1+$G$162)^2</f>
+        <v/>
+      </c>
+      <c r="I174" s="11">
+        <f>1/(1+$G$162)^3</f>
+        <v/>
+      </c>
+      <c r="J174" s="11">
+        <f>1/(1+$G$162)^4</f>
+        <v/>
+      </c>
+      <c r="K174" s="11">
+        <f>1/(1+$G$162)^5</f>
+        <v/>
+      </c>
+      <c r="L174" s="11">
+        <f>1/(1+$G$162)^6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="175">
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>PV of FCF</t>
+        </is>
+      </c>
+      <c r="G175" s="3">
+        <f>G171*G174</f>
+        <v/>
+      </c>
+      <c r="H175" s="3">
+        <f>H171*H174</f>
+        <v/>
+      </c>
+      <c r="I175" s="3">
+        <f>I171*I174</f>
+        <v/>
+      </c>
+      <c r="J175" s="3">
+        <f>J171*J174</f>
+        <v/>
+      </c>
+      <c r="K175" s="3">
+        <f>K171*K174</f>
+        <v/>
+      </c>
+      <c r="L175" s="3">
+        <f>L171*L174</f>
+        <v/>
+      </c>
+    </row>
+    <row r="177">
+      <c r="B177" s="2" t="inlineStr">
+        <is>
+          <t>VALUATION SUMMARY</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Sum of PV of FCFs</t>
+        </is>
+      </c>
+      <c r="G178" s="3">
+        <f>G175+H175+I175+J175+K175+L175</f>
+        <v/>
+      </c>
+    </row>
+    <row r="179">
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Terminal Year FCF</t>
+        </is>
+      </c>
+      <c r="G179" s="3">
+        <f>L171</f>
+        <v/>
+      </c>
+    </row>
+    <row r="180">
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Terminal Value (Gordon Growth)</t>
+        </is>
+      </c>
+      <c r="G180" s="3">
+        <f>G179*(1+$G$163)/($G$162-$G$163)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="181">
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>PV of Terminal Value</t>
+        </is>
+      </c>
+      <c r="G181" s="3">
+        <f>G180*L174</f>
+        <v/>
+      </c>
+    </row>
+    <row r="182">
+      <c r="B182" s="5" t="inlineStr">
+        <is>
+          <t>Enterprise Value</t>
+        </is>
+      </c>
+      <c r="G182" s="3">
+        <f>G178+G181</f>
+        <v/>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B185" s="2" t="inlineStr">
+        <is>
+          <t>MARKET DATA &amp; VALUATION COMPARISON</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="B186" s="2" t="inlineStr">
+        <is>
+          <t>MARKET INPUTS (Update Manually)</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="B187" s="9" t="inlineStr">
+        <is>
+          <t>Shares Outstanding (millions)</t>
+        </is>
+      </c>
+      <c r="G187" s="12" t="n">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="B188" s="9" t="inlineStr">
+        <is>
+          <t>Current Stock Price ($)</t>
+        </is>
+      </c>
+      <c r="G188" s="13" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Market Cap (thousands)</t>
+        </is>
+      </c>
+      <c r="G189" s="3">
+        <f>G187*G188*1000</f>
+        <v/>
+      </c>
+    </row>
+    <row r="190">
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Total Debt (FY2024)</t>
+        </is>
+      </c>
+      <c r="G190" s="3">
+        <f>F77</f>
+        <v/>
+      </c>
+    </row>
+    <row r="191">
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Cash (FY2024)</t>
+        </is>
+      </c>
+      <c r="G191" s="3">
+        <f>F46</f>
+        <v/>
+      </c>
+    </row>
+    <row r="192">
+      <c r="B192" s="5" t="inlineStr">
+        <is>
+          <t>Net Debt</t>
+        </is>
+      </c>
+      <c r="G192" s="3">
+        <f>G190-G191</f>
+        <v/>
+      </c>
+    </row>
+    <row r="193">
+      <c r="B193" s="5" t="inlineStr">
+        <is>
+          <t>Current Enterprise Value</t>
+        </is>
+      </c>
+      <c r="G193" s="3">
+        <f>G189+G192</f>
+        <v/>
+      </c>
+    </row>
+    <row r="195">
+      <c r="B195" s="2" t="inlineStr">
+        <is>
+          <t>VALUATION COMPARISON</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>DCF Enterprise Value</t>
+        </is>
+      </c>
+      <c r="G196" s="3">
+        <f>G182</f>
+        <v/>
+      </c>
+    </row>
+    <row r="197">
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Implied Equity Value</t>
+        </is>
+      </c>
+      <c r="G197" s="3">
+        <f>G196-G192</f>
+        <v/>
+      </c>
+    </row>
+    <row r="198">
+      <c r="B198" s="5" t="inlineStr">
+        <is>
+          <t>Implied Share Price ($)</t>
+        </is>
+      </c>
+      <c r="G198" s="14">
+        <f>G197/G187/1000</f>
+        <v/>
+      </c>
+    </row>
+    <row r="199">
+      <c r="B199" s="5" t="inlineStr">
+        <is>
+          <t>Upside / (Downside) %</t>
+        </is>
+      </c>
+      <c r="G199" s="15">
+        <f>G198/G188-1</f>
+        <v/>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B202" s="2" t="inlineStr">
+        <is>
+          <t>DATA SOURCES &amp; FILING REFERENCES</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>SEC EDGAR: https://www.sec.gov/cgi-bin/browse-edgar?action=getcompany&amp;CIK=0001142750</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Company: AMN Healthcare Services Inc (NYSE: AMN)</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>10-K (Annual): Revenue, all IS items, all BS items</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>10-Q (Quarterly): Quarterly IS data, segment revenue</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Source File: Annual data from 10-K filings; Quarterly from 10-Q filings</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>